<commit_message>
UPDATE: modificado excel de cursos y otras mejoras
</commit_message>
<xml_diff>
--- a/excel/curso.xlsx
+++ b/excel/curso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php_isa\Incidencias_EVG\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,78 +26,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
-    <t>ESO1A</t>
-  </si>
-  <si>
     <t>1º de la ESO A</t>
   </si>
   <si>
     <t>ESO</t>
   </si>
   <si>
-    <t>ESO1B</t>
-  </si>
-  <si>
     <t>1º de la ESO B</t>
   </si>
   <si>
-    <t>ESO1C</t>
-  </si>
-  <si>
     <t>1º de la ESO C</t>
   </si>
   <si>
-    <t>ESO2A</t>
-  </si>
-  <si>
     <t>2º de la ESO A</t>
   </si>
   <si>
-    <t>ESO2B</t>
-  </si>
-  <si>
     <t>2º de la ESO B</t>
   </si>
   <si>
-    <t>ESO2C</t>
-  </si>
-  <si>
     <t>2º de la ESO C</t>
   </si>
   <si>
-    <t>ESO3A</t>
-  </si>
-  <si>
     <t>3º de la ESO A</t>
   </si>
   <si>
-    <t>ESO3B</t>
-  </si>
-  <si>
     <t>3º de la ESO B</t>
   </si>
   <si>
-    <t>ESO3C</t>
-  </si>
-  <si>
     <t>3º de la ESO C</t>
   </si>
   <si>
-    <t>ESO4A</t>
-  </si>
-  <si>
     <t>4º de la ESO A</t>
   </si>
   <si>
-    <t>ESO4B</t>
-  </si>
-  <si>
     <t>4º de la ESO B</t>
   </si>
   <si>
-    <t>ESO4C</t>
-  </si>
-  <si>
     <t>4º de la ESO C</t>
   </si>
   <si>
@@ -159,6 +123,42 @@
   </si>
   <si>
     <t>2º de Desarrollo de Aplicaciones Web</t>
+  </si>
+  <si>
+    <t>1ESOA</t>
+  </si>
+  <si>
+    <t>1ESOB</t>
+  </si>
+  <si>
+    <t>1ESOC</t>
+  </si>
+  <si>
+    <t>2ESOA</t>
+  </si>
+  <si>
+    <t>2ESOB</t>
+  </si>
+  <si>
+    <t>2ESOC</t>
+  </si>
+  <si>
+    <t>3ESOA</t>
+  </si>
+  <si>
+    <t>3ESOB</t>
+  </si>
+  <si>
+    <t>3ESOC</t>
+  </si>
+  <si>
+    <t>4ESOA</t>
+  </si>
+  <si>
+    <t>4ESOB</t>
+  </si>
+  <si>
+    <t>4ESOC</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,233 +536,233 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>